<commit_message>
Revising earlier added column
</commit_message>
<xml_diff>
--- a/In-Progress-Transcriptions/Smithsonian-Letters.xlsx
+++ b/In-Progress-Transcriptions/Smithsonian-Letters.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awisnicki2\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blazelivingston/Desktop/Livingstone-files/TEI-Files/In-Progress-Transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1452" yWindow="0" windowWidth="23040" windowHeight="10860"/>
+    <workbookView xWindow="1460" yWindow="460" windowWidth="23040" windowHeight="10860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>liv_000493</t>
   </si>
@@ -87,6 +93,24 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Difficulty</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>low-med</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>med-high</t>
+  </si>
+  <si>
+    <t>medium</t>
   </si>
 </sst>
 </file>
@@ -102,7 +126,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -112,6 +136,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59996337778862885"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -128,9 +158,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -194,9 +225,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -229,9 +260,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -411,36 +442,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.21875" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -448,7 +488,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -456,12 +496,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -469,42 +512,63 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -512,24 +576,36 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>12</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
noted which letters I have completed
</commit_message>
<xml_diff>
--- a/In-Progress-Transcriptions/Smithsonian-Letters.xlsx
+++ b/In-Progress-Transcriptions/Smithsonian-Letters.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>liv_000493</t>
   </si>
@@ -445,7 +445,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -516,6 +516,9 @@
       <c r="A8" t="s">
         <v>8</v>
       </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
       <c r="C8" t="s">
         <v>23</v>
       </c>
@@ -556,6 +559,9 @@
       <c r="A13" t="s">
         <v>10</v>
       </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
       <c r="C13" t="s">
         <v>24</v>
       </c>
@@ -563,6 +569,9 @@
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
       </c>
       <c r="C14" t="s">
         <v>24</v>

</xml_diff>